<commit_message>
Change name in obs files from NDVIModel.Script.NDVI to NDVI.Value
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/FAR DMC W20-03.xlsx
+++ b/Tests/Validation/Wheat/data/FAR DMC W20-03.xlsx
@@ -17,8 +17,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,13 +58,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +517,7 @@
       </c>
       <c r="P1" s="2" t="inlineStr">
         <is>
-          <t>NDVIModel.Script.NDVI</t>
+          <t>NDVI.Value</t>
         </is>
       </c>
       <c r="Q1" s="2" t="inlineStr">
@@ -571,7 +572,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -608,7 +609,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -645,7 +646,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>44027</v>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -682,7 +683,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -719,7 +720,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="4" t="n">
         <v>44053</v>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -756,7 +757,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -793,7 +794,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -830,7 +831,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -867,7 +868,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -904,7 +905,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -941,7 +942,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -982,7 +983,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -1051,7 +1052,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -1088,7 +1089,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -1125,7 +1126,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="4" t="n">
         <v>44027</v>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1162,7 +1163,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -1199,7 +1200,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="4" t="n">
         <v>44053</v>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -1236,7 +1237,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -1273,7 +1274,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -1310,7 +1311,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -1347,7 +1348,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -1384,7 +1385,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -1421,7 +1422,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C24" t="inlineStr">
@@ -1462,7 +1463,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C25" t="inlineStr">
@@ -1531,7 +1532,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -1568,7 +1569,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -1605,7 +1606,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="4" t="n">
         <v>44027</v>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -1642,7 +1643,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B29" s="3" t="n">
+      <c r="B29" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -1679,7 +1680,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B30" s="3" t="n">
+      <c r="B30" s="4" t="n">
         <v>44053</v>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -1716,7 +1717,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B31" s="3" t="n">
+      <c r="B31" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -1753,7 +1754,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B32" s="3" t="n">
+      <c r="B32" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -1790,7 +1791,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B33" s="3" t="n">
+      <c r="B33" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -1827,7 +1828,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B34" s="3" t="n">
+      <c r="B34" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -1864,7 +1865,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B35" s="3" t="n">
+      <c r="B35" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -1901,7 +1902,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B36" s="3" t="n">
+      <c r="B36" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C36" t="inlineStr">
@@ -1942,7 +1943,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B37" s="3" t="n">
+      <c r="B37" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C37" t="inlineStr">
@@ -2011,7 +2012,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B38" s="3" t="n">
+      <c r="B38" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -2048,7 +2049,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B39" s="3" t="n">
+      <c r="B39" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C39" t="inlineStr"/>
@@ -2085,7 +2086,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B40" s="3" t="n">
+      <c r="B40" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -2122,7 +2123,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B41" s="3" t="n">
+      <c r="B41" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -2159,7 +2160,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B42" s="3" t="n">
+      <c r="B42" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -2196,7 +2197,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B43" s="3" t="n">
+      <c r="B43" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C43" t="inlineStr"/>
@@ -2233,7 +2234,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B44" s="3" t="n">
+      <c r="B44" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -2270,7 +2271,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B45" s="3" t="n">
+      <c r="B45" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -2307,7 +2308,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B46" s="3" t="n">
+      <c r="B46" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C46" t="inlineStr">
@@ -2348,7 +2349,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B47" s="3" t="n">
+      <c r="B47" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C47" t="inlineStr">
@@ -2417,7 +2418,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B48" s="3" t="n">
+      <c r="B48" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -2454,7 +2455,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B49" s="3" t="n">
+      <c r="B49" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -2491,7 +2492,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B50" s="3" t="n">
+      <c r="B50" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -2528,7 +2529,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B51" s="3" t="n">
+      <c r="B51" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -2565,7 +2566,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B52" s="3" t="n">
+      <c r="B52" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -2602,7 +2603,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B53" s="3" t="n">
+      <c r="B53" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -2639,7 +2640,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B54" s="3" t="n">
+      <c r="B54" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C54" t="inlineStr"/>
@@ -2676,7 +2677,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B55" s="3" t="n">
+      <c r="B55" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C55" t="inlineStr"/>
@@ -2713,7 +2714,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B56" s="3" t="n">
+      <c r="B56" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C56" t="inlineStr">
@@ -2754,7 +2755,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B57" s="3" t="n">
+      <c r="B57" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C57" t="inlineStr">
@@ -2823,7 +2824,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B58" s="3" t="n">
+      <c r="B58" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C58" t="inlineStr"/>
@@ -2860,7 +2861,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B59" s="3" t="n">
+      <c r="B59" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C59" t="inlineStr"/>
@@ -2897,7 +2898,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B60" s="3" t="n">
+      <c r="B60" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C60" t="inlineStr"/>
@@ -2934,7 +2935,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B61" s="3" t="n">
+      <c r="B61" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C61" t="inlineStr"/>
@@ -2971,7 +2972,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B62" s="3" t="n">
+      <c r="B62" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C62" t="inlineStr"/>
@@ -3008,7 +3009,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B63" s="3" t="n">
+      <c r="B63" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C63" t="inlineStr"/>
@@ -3045,7 +3046,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B64" s="3" t="n">
+      <c r="B64" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C64" t="inlineStr"/>
@@ -3082,7 +3083,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B65" s="3" t="n">
+      <c r="B65" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C65" t="inlineStr"/>
@@ -3119,7 +3120,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B66" s="3" t="n">
+      <c r="B66" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C66" t="inlineStr">
@@ -3160,7 +3161,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B67" s="3" t="n">
+      <c r="B67" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C67" t="inlineStr">
@@ -3229,7 +3230,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B68" s="3" t="n">
+      <c r="B68" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -3266,7 +3267,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B69" s="3" t="n">
+      <c r="B69" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -3303,7 +3304,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B70" s="3" t="n">
+      <c r="B70" s="4" t="n">
         <v>44027</v>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -3340,7 +3341,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B71" s="3" t="n">
+      <c r="B71" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C71" t="inlineStr"/>
@@ -3377,7 +3378,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B72" s="3" t="n">
+      <c r="B72" s="4" t="n">
         <v>44053</v>
       </c>
       <c r="C72" t="inlineStr"/>
@@ -3414,7 +3415,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B73" s="3" t="n">
+      <c r="B73" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C73" t="inlineStr"/>
@@ -3451,7 +3452,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B74" s="3" t="n">
+      <c r="B74" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C74" t="inlineStr"/>
@@ -3488,7 +3489,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B75" s="3" t="n">
+      <c r="B75" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C75" t="inlineStr"/>
@@ -3525,7 +3526,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B76" s="3" t="n">
+      <c r="B76" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C76" t="inlineStr"/>
@@ -3562,7 +3563,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B77" s="3" t="n">
+      <c r="B77" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C77" t="inlineStr"/>
@@ -3599,7 +3600,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B78" s="3" t="n">
+      <c r="B78" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C78" t="inlineStr">
@@ -3640,7 +3641,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B79" s="3" t="n">
+      <c r="B79" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C79" t="inlineStr">
@@ -3709,7 +3710,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B80" s="3" t="n">
+      <c r="B80" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C80" t="inlineStr"/>
@@ -3746,7 +3747,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B81" s="3" t="n">
+      <c r="B81" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -3783,7 +3784,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B82" s="3" t="n">
+      <c r="B82" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C82" t="inlineStr"/>
@@ -3820,7 +3821,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B83" s="3" t="n">
+      <c r="B83" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -3857,7 +3858,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B84" s="3" t="n">
+      <c r="B84" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -3894,7 +3895,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B85" s="3" t="n">
+      <c r="B85" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -3931,7 +3932,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B86" s="3" t="n">
+      <c r="B86" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -3968,7 +3969,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B87" s="3" t="n">
+      <c r="B87" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -4005,7 +4006,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B88" s="3" t="n">
+      <c r="B88" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C88" t="inlineStr">
@@ -4046,7 +4047,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B89" s="3" t="n">
+      <c r="B89" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C89" t="inlineStr">
@@ -4115,7 +4116,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B90" s="3" t="n">
+      <c r="B90" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -4152,7 +4153,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B91" s="3" t="n">
+      <c r="B91" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -4189,7 +4190,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B92" s="3" t="n">
+      <c r="B92" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -4226,7 +4227,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B93" s="3" t="n">
+      <c r="B93" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C93" t="inlineStr"/>
@@ -4263,7 +4264,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B94" s="3" t="n">
+      <c r="B94" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C94" t="inlineStr"/>
@@ -4300,7 +4301,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B95" s="3" t="n">
+      <c r="B95" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C95" t="inlineStr"/>
@@ -4337,7 +4338,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B96" s="3" t="n">
+      <c r="B96" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C96" t="inlineStr"/>
@@ -4374,7 +4375,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B97" s="3" t="n">
+      <c r="B97" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C97" t="inlineStr"/>
@@ -4411,7 +4412,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B98" s="3" t="n">
+      <c r="B98" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C98" t="inlineStr">
@@ -4452,7 +4453,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B99" s="3" t="n">
+      <c r="B99" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C99" t="inlineStr">
@@ -4521,7 +4522,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B100" s="3" t="n">
+      <c r="B100" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C100" t="inlineStr"/>
@@ -4558,7 +4559,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B101" s="3" t="n">
+      <c r="B101" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C101" t="inlineStr"/>
@@ -4595,7 +4596,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B102" s="3" t="n">
+      <c r="B102" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C102" t="inlineStr"/>
@@ -4632,7 +4633,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B103" s="3" t="n">
+      <c r="B103" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C103" t="inlineStr"/>
@@ -4669,7 +4670,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B104" s="3" t="n">
+      <c r="B104" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C104" t="inlineStr"/>
@@ -4706,7 +4707,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B105" s="3" t="n">
+      <c r="B105" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C105" t="inlineStr"/>
@@ -4743,7 +4744,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B106" s="3" t="n">
+      <c r="B106" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C106" t="inlineStr"/>
@@ -4780,7 +4781,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B107" s="3" t="n">
+      <c r="B107" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C107" t="inlineStr"/>
@@ -4817,7 +4818,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B108" s="3" t="n">
+      <c r="B108" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C108" t="inlineStr">
@@ -4858,7 +4859,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B109" s="3" t="n">
+      <c r="B109" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C109" t="inlineStr">
@@ -4927,7 +4928,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B110" s="3" t="n">
+      <c r="B110" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -4964,7 +4965,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B111" s="3" t="n">
+      <c r="B111" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -5001,7 +5002,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B112" s="3" t="n">
+      <c r="B112" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -5038,7 +5039,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B113" s="3" t="n">
+      <c r="B113" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C113" t="inlineStr"/>
@@ -5075,7 +5076,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B114" s="3" t="n">
+      <c r="B114" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C114" t="inlineStr"/>
@@ -5112,7 +5113,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B115" s="3" t="n">
+      <c r="B115" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C115" t="inlineStr"/>
@@ -5149,7 +5150,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B116" s="3" t="n">
+      <c r="B116" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -5186,7 +5187,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B117" s="3" t="n">
+      <c r="B117" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C117" t="inlineStr">
@@ -5227,7 +5228,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B118" s="3" t="n">
+      <c r="B118" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C118" t="inlineStr">
@@ -5296,7 +5297,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B119" s="3" t="n">
+      <c r="B119" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C119" t="inlineStr"/>
@@ -5333,7 +5334,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B120" s="3" t="n">
+      <c r="B120" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C120" t="inlineStr"/>
@@ -5370,7 +5371,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B121" s="3" t="n">
+      <c r="B121" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C121" t="inlineStr"/>
@@ -5407,7 +5408,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B122" s="3" t="n">
+      <c r="B122" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C122" t="inlineStr"/>
@@ -5444,7 +5445,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B123" s="3" t="n">
+      <c r="B123" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C123" t="inlineStr"/>
@@ -5481,7 +5482,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B124" s="3" t="n">
+      <c r="B124" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C124" t="inlineStr"/>
@@ -5518,7 +5519,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B125" s="3" t="n">
+      <c r="B125" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -5555,7 +5556,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B126" s="3" t="n">
+      <c r="B126" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C126" t="inlineStr">
@@ -5596,7 +5597,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B127" s="3" t="n">
+      <c r="B127" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C127" t="inlineStr">
@@ -5665,7 +5666,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B128" s="3" t="n">
+      <c r="B128" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C128" t="inlineStr"/>
@@ -5702,7 +5703,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B129" s="3" t="n">
+      <c r="B129" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -5739,7 +5740,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B130" s="3" t="n">
+      <c r="B130" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C130" t="inlineStr"/>
@@ -5776,7 +5777,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B131" s="3" t="n">
+      <c r="B131" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -5813,7 +5814,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B132" s="3" t="n">
+      <c r="B132" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C132" t="inlineStr"/>
@@ -5850,7 +5851,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B133" s="3" t="n">
+      <c r="B133" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C133" t="inlineStr"/>
@@ -5887,7 +5888,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B134" s="3" t="n">
+      <c r="B134" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C134" t="inlineStr"/>
@@ -5924,7 +5925,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B135" s="3" t="n">
+      <c r="B135" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C135" t="inlineStr">
@@ -5965,7 +5966,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B136" s="3" t="n">
+      <c r="B136" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C136" t="inlineStr">
@@ -6034,7 +6035,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B137" s="3" t="n">
+      <c r="B137" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -6071,7 +6072,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B138" s="3" t="n">
+      <c r="B138" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C138" t="inlineStr"/>
@@ -6108,7 +6109,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B139" s="3" t="n">
+      <c r="B139" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C139" t="inlineStr"/>
@@ -6145,7 +6146,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B140" s="3" t="n">
+      <c r="B140" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C140" t="inlineStr"/>
@@ -6182,7 +6183,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B141" s="3" t="n">
+      <c r="B141" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C141" t="inlineStr"/>
@@ -6219,7 +6220,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B142" s="3" t="n">
+      <c r="B142" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C142" t="inlineStr"/>
@@ -6256,7 +6257,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B143" s="3" t="n">
+      <c r="B143" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C143" t="inlineStr"/>
@@ -6293,7 +6294,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B144" s="3" t="n">
+      <c r="B144" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C144" t="inlineStr">
@@ -6334,7 +6335,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B145" s="3" t="n">
+      <c r="B145" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C145" t="inlineStr">
@@ -6403,7 +6404,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B146" s="3" t="n">
+      <c r="B146" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C146" t="inlineStr"/>
@@ -6440,7 +6441,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B147" s="3" t="n">
+      <c r="B147" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C147" t="inlineStr"/>
@@ -6477,7 +6478,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B148" s="3" t="n">
+      <c r="B148" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -6514,7 +6515,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B149" s="3" t="n">
+      <c r="B149" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C149" t="inlineStr"/>
@@ -6551,7 +6552,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B150" s="3" t="n">
+      <c r="B150" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C150" t="inlineStr"/>
@@ -6588,7 +6589,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B151" s="3" t="n">
+      <c r="B151" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C151" t="inlineStr"/>
@@ -6625,7 +6626,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B152" s="3" t="n">
+      <c r="B152" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C152" t="inlineStr"/>
@@ -6662,7 +6663,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B153" s="3" t="n">
+      <c r="B153" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C153" t="inlineStr">
@@ -6703,7 +6704,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B154" s="3" t="n">
+      <c r="B154" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C154" t="inlineStr">
@@ -6772,7 +6773,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B155" s="3" t="n">
+      <c r="B155" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C155" t="inlineStr"/>
@@ -6809,7 +6810,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B156" s="3" t="n">
+      <c r="B156" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C156" t="inlineStr"/>
@@ -6846,7 +6847,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B157" s="3" t="n">
+      <c r="B157" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C157" t="inlineStr"/>
@@ -6883,7 +6884,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B158" s="3" t="n">
+      <c r="B158" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C158" t="inlineStr"/>
@@ -6920,7 +6921,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B159" s="3" t="n">
+      <c r="B159" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C159" t="inlineStr"/>
@@ -6957,7 +6958,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B160" s="3" t="n">
+      <c r="B160" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C160" t="inlineStr"/>
@@ -6994,7 +6995,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B161" s="3" t="n">
+      <c r="B161" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C161" t="inlineStr"/>
@@ -7031,7 +7032,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B162" s="3" t="n">
+      <c r="B162" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C162" t="inlineStr">
@@ -7072,7 +7073,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B163" s="3" t="n">
+      <c r="B163" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C163" t="inlineStr">
@@ -7141,7 +7142,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B164" s="3" t="n">
+      <c r="B164" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C164" t="inlineStr"/>
@@ -7178,7 +7179,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B165" s="3" t="n">
+      <c r="B165" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C165" t="inlineStr"/>
@@ -7215,7 +7216,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B166" s="3" t="n">
+      <c r="B166" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C166" t="inlineStr"/>
@@ -7252,7 +7253,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B167" s="3" t="n">
+      <c r="B167" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C167" t="inlineStr"/>
@@ -7289,7 +7290,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B168" s="3" t="n">
+      <c r="B168" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C168" t="inlineStr"/>
@@ -7326,7 +7327,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B169" s="3" t="n">
+      <c r="B169" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C169" t="inlineStr"/>
@@ -7363,7 +7364,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B170" s="3" t="n">
+      <c r="B170" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C170" t="inlineStr"/>
@@ -7400,7 +7401,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B171" s="3" t="n">
+      <c r="B171" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C171" t="inlineStr">
@@ -7441,7 +7442,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B172" s="3" t="n">
+      <c r="B172" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C172" t="inlineStr">
@@ -7510,7 +7511,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B173" s="3" t="n">
+      <c r="B173" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C173" t="inlineStr"/>
@@ -7547,7 +7548,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B174" s="3" t="n">
+      <c r="B174" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C174" t="inlineStr"/>
@@ -7584,7 +7585,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B175" s="3" t="n">
+      <c r="B175" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C175" t="inlineStr"/>
@@ -7621,7 +7622,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B176" s="3" t="n">
+      <c r="B176" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C176" t="inlineStr"/>
@@ -7658,7 +7659,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B177" s="3" t="n">
+      <c r="B177" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C177" t="inlineStr"/>
@@ -7695,7 +7696,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B178" s="3" t="n">
+      <c r="B178" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C178" t="inlineStr"/>
@@ -7732,7 +7733,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B179" s="3" t="n">
+      <c r="B179" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C179" t="inlineStr"/>
@@ -7769,7 +7770,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B180" s="3" t="n">
+      <c r="B180" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C180" t="inlineStr">
@@ -7810,7 +7811,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B181" s="3" t="n">
+      <c r="B181" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C181" t="inlineStr">
@@ -7879,7 +7880,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B182" s="3" t="n">
+      <c r="B182" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C182" t="inlineStr"/>
@@ -7916,7 +7917,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B183" s="3" t="n">
+      <c r="B183" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C183" t="inlineStr"/>
@@ -7953,7 +7954,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B184" s="3" t="n">
+      <c r="B184" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C184" t="inlineStr"/>
@@ -7990,7 +7991,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B185" s="3" t="n">
+      <c r="B185" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C185" t="inlineStr"/>
@@ -8027,7 +8028,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B186" s="3" t="n">
+      <c r="B186" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C186" t="inlineStr"/>
@@ -8064,7 +8065,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B187" s="3" t="n">
+      <c r="B187" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C187" t="inlineStr"/>
@@ -8101,7 +8102,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B188" s="3" t="n">
+      <c r="B188" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C188" t="inlineStr"/>
@@ -8138,7 +8139,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B189" s="3" t="n">
+      <c r="B189" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C189" t="inlineStr">
@@ -8179,7 +8180,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B190" s="3" t="n">
+      <c r="B190" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C190" t="inlineStr">
@@ -8248,7 +8249,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B191" s="3" t="n">
+      <c r="B191" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C191" t="inlineStr"/>
@@ -8285,7 +8286,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B192" s="3" t="n">
+      <c r="B192" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C192" t="inlineStr"/>
@@ -8322,7 +8323,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B193" s="3" t="n">
+      <c r="B193" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C193" t="inlineStr"/>
@@ -8359,7 +8360,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B194" s="3" t="n">
+      <c r="B194" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C194" t="inlineStr"/>
@@ -8396,7 +8397,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B195" s="3" t="n">
+      <c r="B195" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C195" t="inlineStr"/>
@@ -8433,7 +8434,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B196" s="3" t="n">
+      <c r="B196" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C196" t="inlineStr"/>
@@ -8470,7 +8471,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B197" s="3" t="n">
+      <c r="B197" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C197" t="inlineStr"/>
@@ -8507,7 +8508,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B198" s="3" t="n">
+      <c r="B198" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C198" t="inlineStr">
@@ -8548,7 +8549,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B199" s="3" t="n">
+      <c r="B199" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C199" t="inlineStr">
@@ -8617,7 +8618,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B200" s="3" t="n">
+      <c r="B200" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C200" t="inlineStr"/>
@@ -8654,7 +8655,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B201" s="3" t="n">
+      <c r="B201" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -8691,7 +8692,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B202" s="3" t="n">
+      <c r="B202" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -8728,7 +8729,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B203" s="3" t="n">
+      <c r="B203" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C203" t="inlineStr"/>
@@ -8765,7 +8766,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B204" s="3" t="n">
+      <c r="B204" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -8802,7 +8803,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B205" s="3" t="n">
+      <c r="B205" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C205" t="inlineStr"/>
@@ -8839,7 +8840,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B206" s="3" t="n">
+      <c r="B206" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C206" t="inlineStr"/>
@@ -8876,7 +8877,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B207" s="3" t="n">
+      <c r="B207" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C207" t="inlineStr">
@@ -8917,7 +8918,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B208" s="3" t="n">
+      <c r="B208" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C208" t="inlineStr">
@@ -8986,7 +8987,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B209" s="3" t="n">
+      <c r="B209" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C209" t="inlineStr"/>
@@ -9023,7 +9024,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B210" s="3" t="n">
+      <c r="B210" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C210" t="inlineStr"/>
@@ -9060,7 +9061,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B211" s="3" t="n">
+      <c r="B211" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C211" t="inlineStr"/>
@@ -9097,7 +9098,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B212" s="3" t="n">
+      <c r="B212" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C212" t="inlineStr"/>
@@ -9134,7 +9135,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B213" s="3" t="n">
+      <c r="B213" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C213" t="inlineStr"/>
@@ -9171,7 +9172,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B214" s="3" t="n">
+      <c r="B214" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C214" t="inlineStr"/>
@@ -9208,7 +9209,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B215" s="3" t="n">
+      <c r="B215" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C215" t="inlineStr"/>
@@ -9245,7 +9246,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B216" s="3" t="n">
+      <c r="B216" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C216" t="inlineStr">
@@ -9286,7 +9287,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B217" s="3" t="n">
+      <c r="B217" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C217" t="inlineStr">
@@ -9355,7 +9356,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B218" s="3" t="n">
+      <c r="B218" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C218" t="inlineStr"/>
@@ -9392,7 +9393,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B219" s="3" t="n">
+      <c r="B219" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C219" t="inlineStr"/>
@@ -9429,7 +9430,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B220" s="3" t="n">
+      <c r="B220" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C220" t="inlineStr"/>
@@ -9466,7 +9467,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B221" s="3" t="n">
+      <c r="B221" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C221" t="inlineStr"/>
@@ -9503,7 +9504,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B222" s="3" t="n">
+      <c r="B222" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C222" t="inlineStr"/>
@@ -9540,7 +9541,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B223" s="3" t="n">
+      <c r="B223" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C223" t="inlineStr"/>
@@ -9577,7 +9578,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B224" s="3" t="n">
+      <c r="B224" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C224" t="inlineStr"/>
@@ -9614,7 +9615,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B225" s="3" t="n">
+      <c r="B225" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C225" t="inlineStr">
@@ -9655,7 +9656,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B226" s="3" t="n">
+      <c r="B226" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C226" t="inlineStr">
@@ -9724,7 +9725,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B227" s="3" t="n">
+      <c r="B227" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C227" t="inlineStr"/>
@@ -9761,7 +9762,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B228" s="3" t="n">
+      <c r="B228" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C228" t="inlineStr"/>
@@ -9798,7 +9799,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B229" s="3" t="n">
+      <c r="B229" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C229" t="inlineStr"/>
@@ -9835,7 +9836,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B230" s="3" t="n">
+      <c r="B230" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C230" t="inlineStr"/>
@@ -9872,7 +9873,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B231" s="3" t="n">
+      <c r="B231" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C231" t="inlineStr"/>
@@ -9909,7 +9910,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B232" s="3" t="n">
+      <c r="B232" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C232" t="inlineStr"/>
@@ -9946,7 +9947,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B233" s="3" t="n">
+      <c r="B233" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C233" t="inlineStr"/>
@@ -9983,7 +9984,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B234" s="3" t="n">
+      <c r="B234" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C234" t="inlineStr">
@@ -10024,7 +10025,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B235" s="3" t="n">
+      <c r="B235" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C235" t="inlineStr">
@@ -10093,7 +10094,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B236" s="3" t="n">
+      <c r="B236" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C236" t="inlineStr"/>
@@ -10130,7 +10131,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B237" s="3" t="n">
+      <c r="B237" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C237" t="inlineStr"/>
@@ -10167,7 +10168,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B238" s="3" t="n">
+      <c r="B238" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C238" t="inlineStr"/>
@@ -10204,7 +10205,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B239" s="3" t="n">
+      <c r="B239" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C239" t="inlineStr"/>
@@ -10241,7 +10242,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B240" s="3" t="n">
+      <c r="B240" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C240" t="inlineStr"/>
@@ -10278,7 +10279,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B241" s="3" t="n">
+      <c r="B241" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C241" t="inlineStr"/>
@@ -10315,7 +10316,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B242" s="3" t="n">
+      <c r="B242" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C242" t="inlineStr"/>
@@ -10352,7 +10353,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B243" s="3" t="n">
+      <c r="B243" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C243" t="inlineStr">
@@ -10393,7 +10394,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B244" s="3" t="n">
+      <c r="B244" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C244" t="inlineStr">
@@ -10462,7 +10463,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B245" s="3" t="n">
+      <c r="B245" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C245" t="inlineStr"/>
@@ -10499,7 +10500,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B246" s="3" t="n">
+      <c r="B246" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C246" t="inlineStr"/>
@@ -10536,7 +10537,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B247" s="3" t="n">
+      <c r="B247" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C247" t="inlineStr"/>
@@ -10573,7 +10574,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B248" s="3" t="n">
+      <c r="B248" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C248" t="inlineStr"/>
@@ -10610,7 +10611,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B249" s="3" t="n">
+      <c r="B249" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C249" t="inlineStr"/>
@@ -10647,7 +10648,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B250" s="3" t="n">
+      <c r="B250" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C250" t="inlineStr"/>
@@ -10684,7 +10685,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B251" s="3" t="n">
+      <c r="B251" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C251" t="inlineStr"/>
@@ -10721,7 +10722,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B252" s="3" t="n">
+      <c r="B252" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C252" t="inlineStr">
@@ -10762,7 +10763,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B253" s="3" t="n">
+      <c r="B253" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C253" t="inlineStr">
@@ -10831,7 +10832,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B254" s="3" t="n">
+      <c r="B254" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C254" t="inlineStr"/>
@@ -10868,7 +10869,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B255" s="3" t="n">
+      <c r="B255" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C255" t="inlineStr"/>
@@ -10905,7 +10906,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B256" s="3" t="n">
+      <c r="B256" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C256" t="inlineStr"/>
@@ -10942,7 +10943,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B257" s="3" t="n">
+      <c r="B257" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C257" t="inlineStr"/>
@@ -10979,7 +10980,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B258" s="3" t="n">
+      <c r="B258" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C258" t="inlineStr"/>
@@ -11016,7 +11017,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B259" s="3" t="n">
+      <c r="B259" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C259" t="inlineStr"/>
@@ -11053,7 +11054,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B260" s="3" t="n">
+      <c r="B260" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C260" t="inlineStr"/>
@@ -11090,7 +11091,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B261" s="3" t="n">
+      <c r="B261" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C261" t="inlineStr">
@@ -11131,7 +11132,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B262" s="3" t="n">
+      <c r="B262" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C262" t="inlineStr">
@@ -11200,7 +11201,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B263" s="3" t="n">
+      <c r="B263" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C263" t="inlineStr"/>
@@ -11237,7 +11238,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B264" s="3" t="n">
+      <c r="B264" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C264" t="inlineStr"/>
@@ -11274,7 +11275,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B265" s="3" t="n">
+      <c r="B265" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C265" t="inlineStr"/>
@@ -11311,7 +11312,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B266" s="3" t="n">
+      <c r="B266" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C266" t="inlineStr"/>
@@ -11348,7 +11349,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B267" s="3" t="n">
+      <c r="B267" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C267" t="inlineStr"/>
@@ -11385,7 +11386,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B268" s="3" t="n">
+      <c r="B268" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C268" t="inlineStr"/>
@@ -11422,7 +11423,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B269" s="3" t="n">
+      <c r="B269" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C269" t="inlineStr"/>
@@ -11459,7 +11460,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B270" s="3" t="n">
+      <c r="B270" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C270" t="inlineStr">
@@ -11500,7 +11501,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B271" s="3" t="n">
+      <c r="B271" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C271" t="inlineStr">
@@ -11569,7 +11570,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B272" s="3" t="n">
+      <c r="B272" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C272" t="inlineStr"/>
@@ -11606,7 +11607,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B273" s="3" t="n">
+      <c r="B273" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C273" t="inlineStr"/>
@@ -11643,7 +11644,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B274" s="3" t="n">
+      <c r="B274" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C274" t="inlineStr"/>
@@ -11680,7 +11681,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B275" s="3" t="n">
+      <c r="B275" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C275" t="inlineStr"/>
@@ -11717,7 +11718,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B276" s="3" t="n">
+      <c r="B276" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C276" t="inlineStr"/>
@@ -11754,7 +11755,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B277" s="3" t="n">
+      <c r="B277" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C277" t="inlineStr"/>
@@ -11791,7 +11792,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B278" s="3" t="n">
+      <c r="B278" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C278" t="inlineStr"/>
@@ -11828,7 +11829,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B279" s="3" t="n">
+      <c r="B279" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C279" t="inlineStr">
@@ -11869,7 +11870,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B280" s="3" t="n">
+      <c r="B280" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C280" t="inlineStr">
@@ -11938,7 +11939,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B281" s="3" t="n">
+      <c r="B281" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C281" t="inlineStr"/>
@@ -11975,7 +11976,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B282" s="3" t="n">
+      <c r="B282" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C282" t="inlineStr"/>
@@ -12012,7 +12013,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B283" s="3" t="n">
+      <c r="B283" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C283" t="inlineStr"/>
@@ -12049,7 +12050,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B284" s="3" t="n">
+      <c r="B284" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C284" t="inlineStr"/>
@@ -12086,7 +12087,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B285" s="3" t="n">
+      <c r="B285" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C285" t="inlineStr"/>
@@ -12123,7 +12124,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B286" s="3" t="n">
+      <c r="B286" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C286" t="inlineStr"/>
@@ -12160,7 +12161,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B287" s="3" t="n">
+      <c r="B287" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C287" t="inlineStr"/>
@@ -12197,7 +12198,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B288" s="3" t="n">
+      <c r="B288" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C288" t="inlineStr">
@@ -12238,7 +12239,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B289" s="3" t="n">
+      <c r="B289" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C289" t="inlineStr">

</xml_diff>

<commit_message>
Revert obs and wheat.apsimx back to master versions to avoid conflicts
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/FAR DMC W20-03.xlsx
+++ b/Tests/Validation/Wheat/data/FAR DMC W20-03.xlsx
@@ -17,8 +17,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,14 +58,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,7 +516,7 @@
       </c>
       <c r="P1" s="2" t="inlineStr">
         <is>
-          <t>NDVI.Value</t>
+          <t>NDVIModel.Script.NDVI</t>
         </is>
       </c>
       <c r="Q1" s="2" t="inlineStr">
@@ -572,7 +571,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -609,7 +608,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -646,7 +645,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="3" t="n">
         <v>44027</v>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -683,7 +682,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -720,7 +719,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="3" t="n">
         <v>44053</v>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -757,7 +756,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -794,7 +793,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -831,7 +830,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -868,7 +867,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -905,7 +904,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -942,7 +941,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -983,7 +982,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B13" s="4" t="n">
+      <c r="B13" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -1052,7 +1051,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B14" s="4" t="n">
+      <c r="B14" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -1089,7 +1088,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B15" s="4" t="n">
+      <c r="B15" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -1126,7 +1125,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B16" s="4" t="n">
+      <c r="B16" s="3" t="n">
         <v>44027</v>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1163,7 +1162,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B17" s="4" t="n">
+      <c r="B17" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -1200,7 +1199,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B18" s="4" t="n">
+      <c r="B18" s="3" t="n">
         <v>44053</v>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -1237,7 +1236,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B19" s="4" t="n">
+      <c r="B19" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -1274,7 +1273,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B20" s="4" t="n">
+      <c r="B20" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -1311,7 +1310,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B21" s="4" t="n">
+      <c r="B21" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -1348,7 +1347,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B22" s="4" t="n">
+      <c r="B22" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -1385,7 +1384,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B23" s="4" t="n">
+      <c r="B23" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -1422,7 +1421,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B24" s="4" t="n">
+      <c r="B24" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C24" t="inlineStr">
@@ -1463,7 +1462,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B25" s="4" t="n">
+      <c r="B25" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C25" t="inlineStr">
@@ -1532,7 +1531,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B26" s="4" t="n">
+      <c r="B26" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -1569,7 +1568,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B27" s="4" t="n">
+      <c r="B27" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -1606,7 +1605,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B28" s="4" t="n">
+      <c r="B28" s="3" t="n">
         <v>44027</v>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -1643,7 +1642,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B29" s="4" t="n">
+      <c r="B29" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -1680,7 +1679,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B30" s="4" t="n">
+      <c r="B30" s="3" t="n">
         <v>44053</v>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -1717,7 +1716,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B31" s="4" t="n">
+      <c r="B31" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -1754,7 +1753,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B32" s="4" t="n">
+      <c r="B32" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -1791,7 +1790,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B33" s="4" t="n">
+      <c r="B33" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -1828,7 +1827,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B34" s="4" t="n">
+      <c r="B34" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -1865,7 +1864,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B35" s="4" t="n">
+      <c r="B35" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -1902,7 +1901,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B36" s="4" t="n">
+      <c r="B36" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C36" t="inlineStr">
@@ -1943,7 +1942,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B37" s="4" t="n">
+      <c r="B37" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C37" t="inlineStr">
@@ -2012,7 +2011,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B38" s="4" t="n">
+      <c r="B38" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -2049,7 +2048,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B39" s="4" t="n">
+      <c r="B39" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C39" t="inlineStr"/>
@@ -2086,7 +2085,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B40" s="4" t="n">
+      <c r="B40" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -2123,7 +2122,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B41" s="4" t="n">
+      <c r="B41" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -2160,7 +2159,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B42" s="4" t="n">
+      <c r="B42" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -2197,7 +2196,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B43" s="4" t="n">
+      <c r="B43" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C43" t="inlineStr"/>
@@ -2234,7 +2233,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B44" s="4" t="n">
+      <c r="B44" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -2271,7 +2270,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B45" s="4" t="n">
+      <c r="B45" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -2308,7 +2307,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B46" s="4" t="n">
+      <c r="B46" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C46" t="inlineStr">
@@ -2349,7 +2348,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B47" s="4" t="n">
+      <c r="B47" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C47" t="inlineStr">
@@ -2418,7 +2417,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B48" s="4" t="n">
+      <c r="B48" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -2455,7 +2454,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B49" s="4" t="n">
+      <c r="B49" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -2492,7 +2491,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B50" s="4" t="n">
+      <c r="B50" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -2529,7 +2528,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B51" s="4" t="n">
+      <c r="B51" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -2566,7 +2565,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B52" s="4" t="n">
+      <c r="B52" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -2603,7 +2602,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B53" s="4" t="n">
+      <c r="B53" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -2640,7 +2639,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B54" s="4" t="n">
+      <c r="B54" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C54" t="inlineStr"/>
@@ -2677,7 +2676,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B55" s="4" t="n">
+      <c r="B55" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C55" t="inlineStr"/>
@@ -2714,7 +2713,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B56" s="4" t="n">
+      <c r="B56" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C56" t="inlineStr">
@@ -2755,7 +2754,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B57" s="4" t="n">
+      <c r="B57" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C57" t="inlineStr">
@@ -2824,7 +2823,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B58" s="4" t="n">
+      <c r="B58" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C58" t="inlineStr"/>
@@ -2861,7 +2860,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B59" s="4" t="n">
+      <c r="B59" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C59" t="inlineStr"/>
@@ -2898,7 +2897,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B60" s="4" t="n">
+      <c r="B60" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C60" t="inlineStr"/>
@@ -2935,7 +2934,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B61" s="4" t="n">
+      <c r="B61" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C61" t="inlineStr"/>
@@ -2972,7 +2971,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B62" s="4" t="n">
+      <c r="B62" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C62" t="inlineStr"/>
@@ -3009,7 +3008,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B63" s="4" t="n">
+      <c r="B63" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C63" t="inlineStr"/>
@@ -3046,7 +3045,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B64" s="4" t="n">
+      <c r="B64" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C64" t="inlineStr"/>
@@ -3083,7 +3082,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B65" s="4" t="n">
+      <c r="B65" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C65" t="inlineStr"/>
@@ -3120,7 +3119,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B66" s="4" t="n">
+      <c r="B66" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C66" t="inlineStr">
@@ -3161,7 +3160,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B67" s="4" t="n">
+      <c r="B67" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C67" t="inlineStr">
@@ -3230,7 +3229,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B68" s="4" t="n">
+      <c r="B68" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -3267,7 +3266,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B69" s="4" t="n">
+      <c r="B69" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -3304,7 +3303,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B70" s="4" t="n">
+      <c r="B70" s="3" t="n">
         <v>44027</v>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -3341,7 +3340,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B71" s="4" t="n">
+      <c r="B71" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C71" t="inlineStr"/>
@@ -3378,7 +3377,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B72" s="4" t="n">
+      <c r="B72" s="3" t="n">
         <v>44053</v>
       </c>
       <c r="C72" t="inlineStr"/>
@@ -3415,7 +3414,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B73" s="4" t="n">
+      <c r="B73" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C73" t="inlineStr"/>
@@ -3452,7 +3451,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B74" s="4" t="n">
+      <c r="B74" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C74" t="inlineStr"/>
@@ -3489,7 +3488,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B75" s="4" t="n">
+      <c r="B75" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C75" t="inlineStr"/>
@@ -3526,7 +3525,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B76" s="4" t="n">
+      <c r="B76" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C76" t="inlineStr"/>
@@ -3563,7 +3562,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B77" s="4" t="n">
+      <c r="B77" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C77" t="inlineStr"/>
@@ -3600,7 +3599,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B78" s="4" t="n">
+      <c r="B78" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C78" t="inlineStr">
@@ -3641,7 +3640,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B79" s="4" t="n">
+      <c r="B79" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C79" t="inlineStr">
@@ -3710,7 +3709,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B80" s="4" t="n">
+      <c r="B80" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C80" t="inlineStr"/>
@@ -3747,7 +3746,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B81" s="4" t="n">
+      <c r="B81" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -3784,7 +3783,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B82" s="4" t="n">
+      <c r="B82" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C82" t="inlineStr"/>
@@ -3821,7 +3820,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B83" s="4" t="n">
+      <c r="B83" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -3858,7 +3857,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B84" s="4" t="n">
+      <c r="B84" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -3895,7 +3894,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B85" s="4" t="n">
+      <c r="B85" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -3932,7 +3931,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B86" s="4" t="n">
+      <c r="B86" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -3969,7 +3968,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B87" s="4" t="n">
+      <c r="B87" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -4006,7 +4005,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B88" s="4" t="n">
+      <c r="B88" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C88" t="inlineStr">
@@ -4047,7 +4046,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B89" s="4" t="n">
+      <c r="B89" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C89" t="inlineStr">
@@ -4116,7 +4115,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B90" s="4" t="n">
+      <c r="B90" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -4153,7 +4152,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B91" s="4" t="n">
+      <c r="B91" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -4190,7 +4189,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B92" s="4" t="n">
+      <c r="B92" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -4227,7 +4226,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B93" s="4" t="n">
+      <c r="B93" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C93" t="inlineStr"/>
@@ -4264,7 +4263,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B94" s="4" t="n">
+      <c r="B94" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C94" t="inlineStr"/>
@@ -4301,7 +4300,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B95" s="4" t="n">
+      <c r="B95" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C95" t="inlineStr"/>
@@ -4338,7 +4337,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B96" s="4" t="n">
+      <c r="B96" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C96" t="inlineStr"/>
@@ -4375,7 +4374,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B97" s="4" t="n">
+      <c r="B97" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C97" t="inlineStr"/>
@@ -4412,7 +4411,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B98" s="4" t="n">
+      <c r="B98" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C98" t="inlineStr">
@@ -4453,7 +4452,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B99" s="4" t="n">
+      <c r="B99" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C99" t="inlineStr">
@@ -4522,7 +4521,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B100" s="4" t="n">
+      <c r="B100" s="3" t="n">
         <v>43979</v>
       </c>
       <c r="C100" t="inlineStr"/>
@@ -4559,7 +4558,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B101" s="4" t="n">
+      <c r="B101" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C101" t="inlineStr"/>
@@ -4596,7 +4595,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B102" s="4" t="n">
+      <c r="B102" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C102" t="inlineStr"/>
@@ -4633,7 +4632,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B103" s="4" t="n">
+      <c r="B103" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C103" t="inlineStr"/>
@@ -4670,7 +4669,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B104" s="4" t="n">
+      <c r="B104" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C104" t="inlineStr"/>
@@ -4707,7 +4706,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B105" s="4" t="n">
+      <c r="B105" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C105" t="inlineStr"/>
@@ -4744,7 +4743,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B106" s="4" t="n">
+      <c r="B106" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C106" t="inlineStr"/>
@@ -4781,7 +4780,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B107" s="4" t="n">
+      <c r="B107" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C107" t="inlineStr"/>
@@ -4818,7 +4817,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B108" s="4" t="n">
+      <c r="B108" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C108" t="inlineStr">
@@ -4859,7 +4858,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B109" s="4" t="n">
+      <c r="B109" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C109" t="inlineStr">
@@ -4928,7 +4927,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B110" s="4" t="n">
+      <c r="B110" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -4965,7 +4964,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B111" s="4" t="n">
+      <c r="B111" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -5002,7 +5001,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B112" s="4" t="n">
+      <c r="B112" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -5039,7 +5038,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B113" s="4" t="n">
+      <c r="B113" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C113" t="inlineStr"/>
@@ -5076,7 +5075,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B114" s="4" t="n">
+      <c r="B114" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C114" t="inlineStr"/>
@@ -5113,7 +5112,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B115" s="4" t="n">
+      <c r="B115" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C115" t="inlineStr"/>
@@ -5150,7 +5149,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B116" s="4" t="n">
+      <c r="B116" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -5187,7 +5186,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B117" s="4" t="n">
+      <c r="B117" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C117" t="inlineStr">
@@ -5228,7 +5227,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B118" s="4" t="n">
+      <c r="B118" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C118" t="inlineStr">
@@ -5297,7 +5296,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B119" s="4" t="n">
+      <c r="B119" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C119" t="inlineStr"/>
@@ -5334,7 +5333,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B120" s="4" t="n">
+      <c r="B120" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C120" t="inlineStr"/>
@@ -5371,7 +5370,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B121" s="4" t="n">
+      <c r="B121" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C121" t="inlineStr"/>
@@ -5408,7 +5407,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B122" s="4" t="n">
+      <c r="B122" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C122" t="inlineStr"/>
@@ -5445,7 +5444,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B123" s="4" t="n">
+      <c r="B123" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C123" t="inlineStr"/>
@@ -5482,7 +5481,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B124" s="4" t="n">
+      <c r="B124" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C124" t="inlineStr"/>
@@ -5519,7 +5518,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B125" s="4" t="n">
+      <c r="B125" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -5556,7 +5555,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B126" s="4" t="n">
+      <c r="B126" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C126" t="inlineStr">
@@ -5597,7 +5596,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B127" s="4" t="n">
+      <c r="B127" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C127" t="inlineStr">
@@ -5666,7 +5665,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B128" s="4" t="n">
+      <c r="B128" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C128" t="inlineStr"/>
@@ -5703,7 +5702,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B129" s="4" t="n">
+      <c r="B129" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -5740,7 +5739,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B130" s="4" t="n">
+      <c r="B130" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C130" t="inlineStr"/>
@@ -5777,7 +5776,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B131" s="4" t="n">
+      <c r="B131" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -5814,7 +5813,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B132" s="4" t="n">
+      <c r="B132" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C132" t="inlineStr"/>
@@ -5851,7 +5850,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B133" s="4" t="n">
+      <c r="B133" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C133" t="inlineStr"/>
@@ -5888,7 +5887,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B134" s="4" t="n">
+      <c r="B134" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C134" t="inlineStr"/>
@@ -5925,7 +5924,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B135" s="4" t="n">
+      <c r="B135" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C135" t="inlineStr">
@@ -5966,7 +5965,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B136" s="4" t="n">
+      <c r="B136" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C136" t="inlineStr">
@@ -6035,7 +6034,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B137" s="4" t="n">
+      <c r="B137" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -6072,7 +6071,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B138" s="4" t="n">
+      <c r="B138" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C138" t="inlineStr"/>
@@ -6109,7 +6108,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B139" s="4" t="n">
+      <c r="B139" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C139" t="inlineStr"/>
@@ -6146,7 +6145,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B140" s="4" t="n">
+      <c r="B140" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C140" t="inlineStr"/>
@@ -6183,7 +6182,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B141" s="4" t="n">
+      <c r="B141" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C141" t="inlineStr"/>
@@ -6220,7 +6219,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B142" s="4" t="n">
+      <c r="B142" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C142" t="inlineStr"/>
@@ -6257,7 +6256,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B143" s="4" t="n">
+      <c r="B143" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C143" t="inlineStr"/>
@@ -6294,7 +6293,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B144" s="4" t="n">
+      <c r="B144" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C144" t="inlineStr">
@@ -6335,7 +6334,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B145" s="4" t="n">
+      <c r="B145" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C145" t="inlineStr">
@@ -6404,7 +6403,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B146" s="4" t="n">
+      <c r="B146" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C146" t="inlineStr"/>
@@ -6441,7 +6440,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B147" s="4" t="n">
+      <c r="B147" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C147" t="inlineStr"/>
@@ -6478,7 +6477,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B148" s="4" t="n">
+      <c r="B148" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -6515,7 +6514,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B149" s="4" t="n">
+      <c r="B149" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C149" t="inlineStr"/>
@@ -6552,7 +6551,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B150" s="4" t="n">
+      <c r="B150" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C150" t="inlineStr"/>
@@ -6589,7 +6588,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B151" s="4" t="n">
+      <c r="B151" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C151" t="inlineStr"/>
@@ -6626,7 +6625,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B152" s="4" t="n">
+      <c r="B152" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C152" t="inlineStr"/>
@@ -6663,7 +6662,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B153" s="4" t="n">
+      <c r="B153" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C153" t="inlineStr">
@@ -6704,7 +6703,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B154" s="4" t="n">
+      <c r="B154" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C154" t="inlineStr">
@@ -6773,7 +6772,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B155" s="4" t="n">
+      <c r="B155" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C155" t="inlineStr"/>
@@ -6810,7 +6809,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B156" s="4" t="n">
+      <c r="B156" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C156" t="inlineStr"/>
@@ -6847,7 +6846,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B157" s="4" t="n">
+      <c r="B157" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C157" t="inlineStr"/>
@@ -6884,7 +6883,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B158" s="4" t="n">
+      <c r="B158" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C158" t="inlineStr"/>
@@ -6921,7 +6920,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B159" s="4" t="n">
+      <c r="B159" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C159" t="inlineStr"/>
@@ -6958,7 +6957,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B160" s="4" t="n">
+      <c r="B160" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C160" t="inlineStr"/>
@@ -6995,7 +6994,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B161" s="4" t="n">
+      <c r="B161" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C161" t="inlineStr"/>
@@ -7032,7 +7031,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B162" s="4" t="n">
+      <c r="B162" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C162" t="inlineStr">
@@ -7073,7 +7072,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B163" s="4" t="n">
+      <c r="B163" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C163" t="inlineStr">
@@ -7142,7 +7141,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B164" s="4" t="n">
+      <c r="B164" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C164" t="inlineStr"/>
@@ -7179,7 +7178,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B165" s="4" t="n">
+      <c r="B165" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C165" t="inlineStr"/>
@@ -7216,7 +7215,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B166" s="4" t="n">
+      <c r="B166" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C166" t="inlineStr"/>
@@ -7253,7 +7252,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B167" s="4" t="n">
+      <c r="B167" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C167" t="inlineStr"/>
@@ -7290,7 +7289,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B168" s="4" t="n">
+      <c r="B168" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C168" t="inlineStr"/>
@@ -7327,7 +7326,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B169" s="4" t="n">
+      <c r="B169" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C169" t="inlineStr"/>
@@ -7364,7 +7363,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B170" s="4" t="n">
+      <c r="B170" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C170" t="inlineStr"/>
@@ -7401,7 +7400,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B171" s="4" t="n">
+      <c r="B171" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C171" t="inlineStr">
@@ -7442,7 +7441,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B172" s="4" t="n">
+      <c r="B172" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C172" t="inlineStr">
@@ -7511,7 +7510,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B173" s="4" t="n">
+      <c r="B173" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C173" t="inlineStr"/>
@@ -7548,7 +7547,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B174" s="4" t="n">
+      <c r="B174" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C174" t="inlineStr"/>
@@ -7585,7 +7584,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B175" s="4" t="n">
+      <c r="B175" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C175" t="inlineStr"/>
@@ -7622,7 +7621,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B176" s="4" t="n">
+      <c r="B176" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C176" t="inlineStr"/>
@@ -7659,7 +7658,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B177" s="4" t="n">
+      <c r="B177" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C177" t="inlineStr"/>
@@ -7696,7 +7695,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B178" s="4" t="n">
+      <c r="B178" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C178" t="inlineStr"/>
@@ -7733,7 +7732,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B179" s="4" t="n">
+      <c r="B179" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C179" t="inlineStr"/>
@@ -7770,7 +7769,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B180" s="4" t="n">
+      <c r="B180" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C180" t="inlineStr">
@@ -7811,7 +7810,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B181" s="4" t="n">
+      <c r="B181" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C181" t="inlineStr">
@@ -7880,7 +7879,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B182" s="4" t="n">
+      <c r="B182" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C182" t="inlineStr"/>
@@ -7917,7 +7916,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B183" s="4" t="n">
+      <c r="B183" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C183" t="inlineStr"/>
@@ -7954,7 +7953,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B184" s="4" t="n">
+      <c r="B184" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C184" t="inlineStr"/>
@@ -7991,7 +7990,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B185" s="4" t="n">
+      <c r="B185" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C185" t="inlineStr"/>
@@ -8028,7 +8027,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B186" s="4" t="n">
+      <c r="B186" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C186" t="inlineStr"/>
@@ -8065,7 +8064,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B187" s="4" t="n">
+      <c r="B187" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C187" t="inlineStr"/>
@@ -8102,7 +8101,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B188" s="4" t="n">
+      <c r="B188" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C188" t="inlineStr"/>
@@ -8139,7 +8138,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B189" s="4" t="n">
+      <c r="B189" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C189" t="inlineStr">
@@ -8180,7 +8179,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B190" s="4" t="n">
+      <c r="B190" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C190" t="inlineStr">
@@ -8249,7 +8248,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B191" s="4" t="n">
+      <c r="B191" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C191" t="inlineStr"/>
@@ -8286,7 +8285,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B192" s="4" t="n">
+      <c r="B192" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C192" t="inlineStr"/>
@@ -8323,7 +8322,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B193" s="4" t="n">
+      <c r="B193" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C193" t="inlineStr"/>
@@ -8360,7 +8359,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B194" s="4" t="n">
+      <c r="B194" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C194" t="inlineStr"/>
@@ -8397,7 +8396,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B195" s="4" t="n">
+      <c r="B195" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C195" t="inlineStr"/>
@@ -8434,7 +8433,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B196" s="4" t="n">
+      <c r="B196" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C196" t="inlineStr"/>
@@ -8471,7 +8470,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B197" s="4" t="n">
+      <c r="B197" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C197" t="inlineStr"/>
@@ -8508,7 +8507,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B198" s="4" t="n">
+      <c r="B198" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C198" t="inlineStr">
@@ -8549,7 +8548,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B199" s="4" t="n">
+      <c r="B199" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C199" t="inlineStr">
@@ -8618,7 +8617,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B200" s="4" t="n">
+      <c r="B200" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C200" t="inlineStr"/>
@@ -8655,7 +8654,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B201" s="4" t="n">
+      <c r="B201" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -8692,7 +8691,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B202" s="4" t="n">
+      <c r="B202" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -8729,7 +8728,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B203" s="4" t="n">
+      <c r="B203" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C203" t="inlineStr"/>
@@ -8766,7 +8765,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B204" s="4" t="n">
+      <c r="B204" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -8803,7 +8802,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B205" s="4" t="n">
+      <c r="B205" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C205" t="inlineStr"/>
@@ -8840,7 +8839,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B206" s="4" t="n">
+      <c r="B206" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C206" t="inlineStr"/>
@@ -8877,7 +8876,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B207" s="4" t="n">
+      <c r="B207" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C207" t="inlineStr">
@@ -8918,7 +8917,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B208" s="4" t="n">
+      <c r="B208" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C208" t="inlineStr">
@@ -8987,7 +8986,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B209" s="4" t="n">
+      <c r="B209" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C209" t="inlineStr"/>
@@ -9024,7 +9023,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B210" s="4" t="n">
+      <c r="B210" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C210" t="inlineStr"/>
@@ -9061,7 +9060,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B211" s="4" t="n">
+      <c r="B211" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C211" t="inlineStr"/>
@@ -9098,7 +9097,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B212" s="4" t="n">
+      <c r="B212" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C212" t="inlineStr"/>
@@ -9135,7 +9134,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B213" s="4" t="n">
+      <c r="B213" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C213" t="inlineStr"/>
@@ -9172,7 +9171,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B214" s="4" t="n">
+      <c r="B214" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C214" t="inlineStr"/>
@@ -9209,7 +9208,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B215" s="4" t="n">
+      <c r="B215" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C215" t="inlineStr"/>
@@ -9246,7 +9245,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B216" s="4" t="n">
+      <c r="B216" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C216" t="inlineStr">
@@ -9287,7 +9286,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B217" s="4" t="n">
+      <c r="B217" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C217" t="inlineStr">
@@ -9356,7 +9355,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B218" s="4" t="n">
+      <c r="B218" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C218" t="inlineStr"/>
@@ -9393,7 +9392,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B219" s="4" t="n">
+      <c r="B219" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C219" t="inlineStr"/>
@@ -9430,7 +9429,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B220" s="4" t="n">
+      <c r="B220" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C220" t="inlineStr"/>
@@ -9467,7 +9466,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B221" s="4" t="n">
+      <c r="B221" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C221" t="inlineStr"/>
@@ -9504,7 +9503,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B222" s="4" t="n">
+      <c r="B222" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C222" t="inlineStr"/>
@@ -9541,7 +9540,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B223" s="4" t="n">
+      <c r="B223" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C223" t="inlineStr"/>
@@ -9578,7 +9577,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B224" s="4" t="n">
+      <c r="B224" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C224" t="inlineStr"/>
@@ -9615,7 +9614,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B225" s="4" t="n">
+      <c r="B225" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C225" t="inlineStr">
@@ -9656,7 +9655,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B226" s="4" t="n">
+      <c r="B226" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C226" t="inlineStr">
@@ -9725,7 +9724,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B227" s="4" t="n">
+      <c r="B227" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C227" t="inlineStr"/>
@@ -9762,7 +9761,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B228" s="4" t="n">
+      <c r="B228" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C228" t="inlineStr"/>
@@ -9799,7 +9798,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B229" s="4" t="n">
+      <c r="B229" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C229" t="inlineStr"/>
@@ -9836,7 +9835,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B230" s="4" t="n">
+      <c r="B230" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C230" t="inlineStr"/>
@@ -9873,7 +9872,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B231" s="4" t="n">
+      <c r="B231" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C231" t="inlineStr"/>
@@ -9910,7 +9909,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B232" s="4" t="n">
+      <c r="B232" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C232" t="inlineStr"/>
@@ -9947,7 +9946,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B233" s="4" t="n">
+      <c r="B233" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C233" t="inlineStr"/>
@@ -9984,7 +9983,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B234" s="4" t="n">
+      <c r="B234" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C234" t="inlineStr">
@@ -10025,7 +10024,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B235" s="4" t="n">
+      <c r="B235" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C235" t="inlineStr">
@@ -10094,7 +10093,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B236" s="4" t="n">
+      <c r="B236" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C236" t="inlineStr"/>
@@ -10131,7 +10130,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B237" s="4" t="n">
+      <c r="B237" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C237" t="inlineStr"/>
@@ -10168,7 +10167,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B238" s="4" t="n">
+      <c r="B238" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C238" t="inlineStr"/>
@@ -10205,7 +10204,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B239" s="4" t="n">
+      <c r="B239" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C239" t="inlineStr"/>
@@ -10242,7 +10241,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B240" s="4" t="n">
+      <c r="B240" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C240" t="inlineStr"/>
@@ -10279,7 +10278,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B241" s="4" t="n">
+      <c r="B241" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C241" t="inlineStr"/>
@@ -10316,7 +10315,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B242" s="4" t="n">
+      <c r="B242" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C242" t="inlineStr"/>
@@ -10353,7 +10352,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B243" s="4" t="n">
+      <c r="B243" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C243" t="inlineStr">
@@ -10394,7 +10393,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B244" s="4" t="n">
+      <c r="B244" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C244" t="inlineStr">
@@ -10463,7 +10462,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B245" s="4" t="n">
+      <c r="B245" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C245" t="inlineStr"/>
@@ -10500,7 +10499,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B246" s="4" t="n">
+      <c r="B246" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C246" t="inlineStr"/>
@@ -10537,7 +10536,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B247" s="4" t="n">
+      <c r="B247" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C247" t="inlineStr"/>
@@ -10574,7 +10573,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B248" s="4" t="n">
+      <c r="B248" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C248" t="inlineStr"/>
@@ -10611,7 +10610,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B249" s="4" t="n">
+      <c r="B249" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C249" t="inlineStr"/>
@@ -10648,7 +10647,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B250" s="4" t="n">
+      <c r="B250" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C250" t="inlineStr"/>
@@ -10685,7 +10684,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B251" s="4" t="n">
+      <c r="B251" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C251" t="inlineStr"/>
@@ -10722,7 +10721,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B252" s="4" t="n">
+      <c r="B252" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C252" t="inlineStr">
@@ -10763,7 +10762,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B253" s="4" t="n">
+      <c r="B253" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C253" t="inlineStr">
@@ -10832,7 +10831,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B254" s="4" t="n">
+      <c r="B254" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C254" t="inlineStr"/>
@@ -10869,7 +10868,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B255" s="4" t="n">
+      <c r="B255" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C255" t="inlineStr"/>
@@ -10906,7 +10905,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B256" s="4" t="n">
+      <c r="B256" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C256" t="inlineStr"/>
@@ -10943,7 +10942,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B257" s="4" t="n">
+      <c r="B257" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C257" t="inlineStr"/>
@@ -10980,7 +10979,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B258" s="4" t="n">
+      <c r="B258" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C258" t="inlineStr"/>
@@ -11017,7 +11016,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B259" s="4" t="n">
+      <c r="B259" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C259" t="inlineStr"/>
@@ -11054,7 +11053,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B260" s="4" t="n">
+      <c r="B260" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C260" t="inlineStr"/>
@@ -11091,7 +11090,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B261" s="4" t="n">
+      <c r="B261" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C261" t="inlineStr">
@@ -11132,7 +11131,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B262" s="4" t="n">
+      <c r="B262" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C262" t="inlineStr">
@@ -11201,7 +11200,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B263" s="4" t="n">
+      <c r="B263" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C263" t="inlineStr"/>
@@ -11238,7 +11237,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B264" s="4" t="n">
+      <c r="B264" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C264" t="inlineStr"/>
@@ -11275,7 +11274,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B265" s="4" t="n">
+      <c r="B265" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C265" t="inlineStr"/>
@@ -11312,7 +11311,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B266" s="4" t="n">
+      <c r="B266" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C266" t="inlineStr"/>
@@ -11349,7 +11348,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B267" s="4" t="n">
+      <c r="B267" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C267" t="inlineStr"/>
@@ -11386,7 +11385,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B268" s="4" t="n">
+      <c r="B268" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C268" t="inlineStr"/>
@@ -11423,7 +11422,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B269" s="4" t="n">
+      <c r="B269" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C269" t="inlineStr"/>
@@ -11460,7 +11459,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B270" s="4" t="n">
+      <c r="B270" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C270" t="inlineStr">
@@ -11501,7 +11500,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B271" s="4" t="n">
+      <c r="B271" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C271" t="inlineStr">
@@ -11570,7 +11569,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B272" s="4" t="n">
+      <c r="B272" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C272" t="inlineStr"/>
@@ -11607,7 +11606,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B273" s="4" t="n">
+      <c r="B273" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C273" t="inlineStr"/>
@@ -11644,7 +11643,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B274" s="4" t="n">
+      <c r="B274" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C274" t="inlineStr"/>
@@ -11681,7 +11680,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B275" s="4" t="n">
+      <c r="B275" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C275" t="inlineStr"/>
@@ -11718,7 +11717,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B276" s="4" t="n">
+      <c r="B276" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C276" t="inlineStr"/>
@@ -11755,7 +11754,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B277" s="4" t="n">
+      <c r="B277" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C277" t="inlineStr"/>
@@ -11792,7 +11791,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B278" s="4" t="n">
+      <c r="B278" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C278" t="inlineStr"/>
@@ -11829,7 +11828,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B279" s="4" t="n">
+      <c r="B279" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C279" t="inlineStr">
@@ -11870,7 +11869,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B280" s="4" t="n">
+      <c r="B280" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C280" t="inlineStr">
@@ -11939,7 +11938,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B281" s="4" t="n">
+      <c r="B281" s="3" t="n">
         <v>44026</v>
       </c>
       <c r="C281" t="inlineStr"/>
@@ -11976,7 +11975,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B282" s="4" t="n">
+      <c r="B282" s="3" t="n">
         <v>44041</v>
       </c>
       <c r="C282" t="inlineStr"/>
@@ -12013,7 +12012,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B283" s="4" t="n">
+      <c r="B283" s="3" t="n">
         <v>44068</v>
       </c>
       <c r="C283" t="inlineStr"/>
@@ -12050,7 +12049,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B284" s="4" t="n">
+      <c r="B284" s="3" t="n">
         <v>44082</v>
       </c>
       <c r="C284" t="inlineStr"/>
@@ -12087,7 +12086,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B285" s="4" t="n">
+      <c r="B285" s="3" t="n">
         <v>44097</v>
       </c>
       <c r="C285" t="inlineStr"/>
@@ -12124,7 +12123,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B286" s="4" t="n">
+      <c r="B286" s="3" t="n">
         <v>44110</v>
       </c>
       <c r="C286" t="inlineStr"/>
@@ -12161,7 +12160,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B287" s="4" t="n">
+      <c r="B287" s="3" t="n">
         <v>44139</v>
       </c>
       <c r="C287" t="inlineStr"/>
@@ -12198,7 +12197,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B288" s="4" t="n">
+      <c r="B288" s="3" t="n">
         <v>44152</v>
       </c>
       <c r="C288" t="inlineStr">
@@ -12239,7 +12238,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B289" s="4" t="n">
+      <c r="B289" s="3" t="n">
         <v>44181</v>
       </c>
       <c r="C289" t="inlineStr">

</xml_diff>

<commit_message>
Convert Manager based NDVI model to compiled model.  Rename NDVI obs
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/FAR DMC W20-03.xlsx
+++ b/Tests/Validation/Wheat/data/FAR DMC W20-03.xlsx
@@ -17,8 +17,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,13 +58,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +517,7 @@
       </c>
       <c r="P1" s="2" t="inlineStr">
         <is>
-          <t>NDVIModel.Script.NDVI</t>
+          <t>Spectral.NDVI</t>
         </is>
       </c>
       <c r="Q1" s="2" t="inlineStr">
@@ -571,7 +572,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -608,7 +609,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -645,7 +646,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="4" t="n">
         <v>44027</v>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -682,7 +683,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -719,7 +720,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="4" t="n">
         <v>44053</v>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -756,7 +757,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -793,7 +794,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -830,7 +831,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -867,7 +868,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -904,7 +905,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -941,7 +942,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -982,7 +983,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTrojan</t>
         </is>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -1051,7 +1052,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -1088,7 +1089,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -1125,7 +1126,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="4" t="n">
         <v>44027</v>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1162,7 +1163,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B17" s="3" t="n">
+      <c r="B17" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -1199,7 +1200,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="4" t="n">
         <v>44053</v>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -1236,7 +1237,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B19" s="3" t="n">
+      <c r="B19" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -1273,7 +1274,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -1310,7 +1311,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -1347,7 +1348,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -1384,7 +1385,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -1421,7 +1422,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B24" s="3" t="n">
+      <c r="B24" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C24" t="inlineStr">
@@ -1462,7 +1463,7 @@
           <t>FAR DMC W20-03MgmtStandardCvScepter</t>
         </is>
       </c>
-      <c r="B25" s="3" t="n">
+      <c r="B25" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C25" t="inlineStr">
@@ -1531,7 +1532,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B26" s="3" t="n">
+      <c r="B26" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -1568,7 +1569,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B27" s="3" t="n">
+      <c r="B27" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -1605,7 +1606,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B28" s="3" t="n">
+      <c r="B28" s="4" t="n">
         <v>44027</v>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -1642,7 +1643,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B29" s="3" t="n">
+      <c r="B29" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -1679,7 +1680,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B30" s="3" t="n">
+      <c r="B30" s="4" t="n">
         <v>44053</v>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -1716,7 +1717,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B31" s="3" t="n">
+      <c r="B31" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -1753,7 +1754,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B32" s="3" t="n">
+      <c r="B32" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -1790,7 +1791,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B33" s="3" t="n">
+      <c r="B33" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -1827,7 +1828,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B34" s="3" t="n">
+      <c r="B34" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -1864,7 +1865,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B35" s="3" t="n">
+      <c r="B35" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -1901,7 +1902,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B36" s="3" t="n">
+      <c r="B36" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C36" t="inlineStr">
@@ -1942,7 +1943,7 @@
           <t>FAR DMC W20-03MgmtStandardCvNighthawk</t>
         </is>
       </c>
-      <c r="B37" s="3" t="n">
+      <c r="B37" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C37" t="inlineStr">
@@ -2011,7 +2012,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B38" s="3" t="n">
+      <c r="B38" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -2048,7 +2049,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B39" s="3" t="n">
+      <c r="B39" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C39" t="inlineStr"/>
@@ -2085,7 +2086,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B40" s="3" t="n">
+      <c r="B40" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -2122,7 +2123,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B41" s="3" t="n">
+      <c r="B41" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -2159,7 +2160,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B42" s="3" t="n">
+      <c r="B42" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -2196,7 +2197,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B43" s="3" t="n">
+      <c r="B43" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C43" t="inlineStr"/>
@@ -2233,7 +2234,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B44" s="3" t="n">
+      <c r="B44" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -2270,7 +2271,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B45" s="3" t="n">
+      <c r="B45" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -2307,7 +2308,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B46" s="3" t="n">
+      <c r="B46" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C46" t="inlineStr">
@@ -2348,7 +2349,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAnapurna</t>
         </is>
       </c>
-      <c r="B47" s="3" t="n">
+      <c r="B47" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C47" t="inlineStr">
@@ -2417,7 +2418,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B48" s="3" t="n">
+      <c r="B48" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -2454,7 +2455,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B49" s="3" t="n">
+      <c r="B49" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -2491,7 +2492,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B50" s="3" t="n">
+      <c r="B50" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -2528,7 +2529,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B51" s="3" t="n">
+      <c r="B51" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -2565,7 +2566,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B52" s="3" t="n">
+      <c r="B52" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -2602,7 +2603,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B53" s="3" t="n">
+      <c r="B53" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -2639,7 +2640,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B54" s="3" t="n">
+      <c r="B54" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C54" t="inlineStr"/>
@@ -2676,7 +2677,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B55" s="3" t="n">
+      <c r="B55" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C55" t="inlineStr"/>
@@ -2713,7 +2714,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B56" s="3" t="n">
+      <c r="B56" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C56" t="inlineStr">
@@ -2754,7 +2755,7 @@
           <t>FAR DMC W20-03MgmtStandardCvAccroc</t>
         </is>
       </c>
-      <c r="B57" s="3" t="n">
+      <c r="B57" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C57" t="inlineStr">
@@ -2823,7 +2824,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B58" s="3" t="n">
+      <c r="B58" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C58" t="inlineStr"/>
@@ -2860,7 +2861,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B59" s="3" t="n">
+      <c r="B59" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C59" t="inlineStr"/>
@@ -2897,7 +2898,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B60" s="3" t="n">
+      <c r="B60" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C60" t="inlineStr"/>
@@ -2934,7 +2935,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B61" s="3" t="n">
+      <c r="B61" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C61" t="inlineStr"/>
@@ -2971,7 +2972,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B62" s="3" t="n">
+      <c r="B62" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C62" t="inlineStr"/>
@@ -3008,7 +3009,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B63" s="3" t="n">
+      <c r="B63" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C63" t="inlineStr"/>
@@ -3045,7 +3046,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B64" s="3" t="n">
+      <c r="B64" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C64" t="inlineStr"/>
@@ -3082,7 +3083,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B65" s="3" t="n">
+      <c r="B65" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C65" t="inlineStr"/>
@@ -3119,7 +3120,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B66" s="3" t="n">
+      <c r="B66" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C66" t="inlineStr">
@@ -3160,7 +3161,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCalabro</t>
         </is>
       </c>
-      <c r="B67" s="3" t="n">
+      <c r="B67" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C67" t="inlineStr">
@@ -3229,7 +3230,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B68" s="3" t="n">
+      <c r="B68" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -3266,7 +3267,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B69" s="3" t="n">
+      <c r="B69" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -3303,7 +3304,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B70" s="3" t="n">
+      <c r="B70" s="4" t="n">
         <v>44027</v>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -3340,7 +3341,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B71" s="3" t="n">
+      <c r="B71" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C71" t="inlineStr"/>
@@ -3377,7 +3378,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B72" s="3" t="n">
+      <c r="B72" s="4" t="n">
         <v>44053</v>
       </c>
       <c r="C72" t="inlineStr"/>
@@ -3414,7 +3415,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B73" s="3" t="n">
+      <c r="B73" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C73" t="inlineStr"/>
@@ -3451,7 +3452,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B74" s="3" t="n">
+      <c r="B74" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C74" t="inlineStr"/>
@@ -3488,7 +3489,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B75" s="3" t="n">
+      <c r="B75" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C75" t="inlineStr"/>
@@ -3525,7 +3526,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B76" s="3" t="n">
+      <c r="B76" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C76" t="inlineStr"/>
@@ -3562,7 +3563,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B77" s="3" t="n">
+      <c r="B77" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C77" t="inlineStr"/>
@@ -3599,7 +3600,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B78" s="3" t="n">
+      <c r="B78" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C78" t="inlineStr">
@@ -3640,7 +3641,7 @@
           <t>FAR DMC W20-03MgmtStandardCvCesario</t>
         </is>
       </c>
-      <c r="B79" s="3" t="n">
+      <c r="B79" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C79" t="inlineStr">
@@ -3709,7 +3710,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B80" s="3" t="n">
+      <c r="B80" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C80" t="inlineStr"/>
@@ -3746,7 +3747,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B81" s="3" t="n">
+      <c r="B81" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -3783,7 +3784,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B82" s="3" t="n">
+      <c r="B82" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C82" t="inlineStr"/>
@@ -3820,7 +3821,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B83" s="3" t="n">
+      <c r="B83" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -3857,7 +3858,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B84" s="3" t="n">
+      <c r="B84" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -3894,7 +3895,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B85" s="3" t="n">
+      <c r="B85" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -3931,7 +3932,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B86" s="3" t="n">
+      <c r="B86" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -3968,7 +3969,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B87" s="3" t="n">
+      <c r="B87" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -4005,7 +4006,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B88" s="3" t="n">
+      <c r="B88" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C88" t="inlineStr">
@@ -4046,7 +4047,7 @@
           <t>FAR DMC W20-03MgmtStandardCvTabasco</t>
         </is>
       </c>
-      <c r="B89" s="3" t="n">
+      <c r="B89" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C89" t="inlineStr">
@@ -4115,7 +4116,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B90" s="3" t="n">
+      <c r="B90" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -4152,7 +4153,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B91" s="3" t="n">
+      <c r="B91" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -4189,7 +4190,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B92" s="3" t="n">
+      <c r="B92" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -4226,7 +4227,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B93" s="3" t="n">
+      <c r="B93" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C93" t="inlineStr"/>
@@ -4263,7 +4264,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B94" s="3" t="n">
+      <c r="B94" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C94" t="inlineStr"/>
@@ -4300,7 +4301,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B95" s="3" t="n">
+      <c r="B95" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C95" t="inlineStr"/>
@@ -4337,7 +4338,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B96" s="3" t="n">
+      <c r="B96" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C96" t="inlineStr"/>
@@ -4374,7 +4375,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B97" s="3" t="n">
+      <c r="B97" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C97" t="inlineStr"/>
@@ -4411,7 +4412,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B98" s="3" t="n">
+      <c r="B98" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C98" t="inlineStr">
@@ -4452,7 +4453,7 @@
           <t>FAR DMC W20-03MgmtStandardCvBennett</t>
         </is>
       </c>
-      <c r="B99" s="3" t="n">
+      <c r="B99" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C99" t="inlineStr">
@@ -4521,7 +4522,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B100" s="3" t="n">
+      <c r="B100" s="4" t="n">
         <v>43979</v>
       </c>
       <c r="C100" t="inlineStr"/>
@@ -4558,7 +4559,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B101" s="3" t="n">
+      <c r="B101" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C101" t="inlineStr"/>
@@ -4595,7 +4596,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B102" s="3" t="n">
+      <c r="B102" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C102" t="inlineStr"/>
@@ -4632,7 +4633,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B103" s="3" t="n">
+      <c r="B103" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C103" t="inlineStr"/>
@@ -4669,7 +4670,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B104" s="3" t="n">
+      <c r="B104" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C104" t="inlineStr"/>
@@ -4706,7 +4707,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B105" s="3" t="n">
+      <c r="B105" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C105" t="inlineStr"/>
@@ -4743,7 +4744,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B106" s="3" t="n">
+      <c r="B106" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C106" t="inlineStr"/>
@@ -4780,7 +4781,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B107" s="3" t="n">
+      <c r="B107" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C107" t="inlineStr"/>
@@ -4817,7 +4818,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B108" s="3" t="n">
+      <c r="B108" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C108" t="inlineStr">
@@ -4858,7 +4859,7 @@
           <t>FAR DMC W20-03MgmtStandardCvManning</t>
         </is>
       </c>
-      <c r="B109" s="3" t="n">
+      <c r="B109" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C109" t="inlineStr">
@@ -4927,7 +4928,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B110" s="3" t="n">
+      <c r="B110" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -4964,7 +4965,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B111" s="3" t="n">
+      <c r="B111" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -5001,7 +5002,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B112" s="3" t="n">
+      <c r="B112" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -5038,7 +5039,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B113" s="3" t="n">
+      <c r="B113" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C113" t="inlineStr"/>
@@ -5075,7 +5076,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B114" s="3" t="n">
+      <c r="B114" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C114" t="inlineStr"/>
@@ -5112,7 +5113,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B115" s="3" t="n">
+      <c r="B115" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C115" t="inlineStr"/>
@@ -5149,7 +5150,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B116" s="3" t="n">
+      <c r="B116" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -5186,7 +5187,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B117" s="3" t="n">
+      <c r="B117" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C117" t="inlineStr">
@@ -5227,7 +5228,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTrojan</t>
         </is>
       </c>
-      <c r="B118" s="3" t="n">
+      <c r="B118" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C118" t="inlineStr">
@@ -5296,7 +5297,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B119" s="3" t="n">
+      <c r="B119" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C119" t="inlineStr"/>
@@ -5333,7 +5334,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B120" s="3" t="n">
+      <c r="B120" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C120" t="inlineStr"/>
@@ -5370,7 +5371,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B121" s="3" t="n">
+      <c r="B121" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C121" t="inlineStr"/>
@@ -5407,7 +5408,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B122" s="3" t="n">
+      <c r="B122" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C122" t="inlineStr"/>
@@ -5444,7 +5445,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B123" s="3" t="n">
+      <c r="B123" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C123" t="inlineStr"/>
@@ -5481,7 +5482,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B124" s="3" t="n">
+      <c r="B124" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C124" t="inlineStr"/>
@@ -5518,7 +5519,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B125" s="3" t="n">
+      <c r="B125" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -5555,7 +5556,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B126" s="3" t="n">
+      <c r="B126" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C126" t="inlineStr">
@@ -5596,7 +5597,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvScepter</t>
         </is>
       </c>
-      <c r="B127" s="3" t="n">
+      <c r="B127" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C127" t="inlineStr">
@@ -5665,7 +5666,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B128" s="3" t="n">
+      <c r="B128" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C128" t="inlineStr"/>
@@ -5702,7 +5703,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B129" s="3" t="n">
+      <c r="B129" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -5739,7 +5740,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B130" s="3" t="n">
+      <c r="B130" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C130" t="inlineStr"/>
@@ -5776,7 +5777,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B131" s="3" t="n">
+      <c r="B131" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -5813,7 +5814,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B132" s="3" t="n">
+      <c r="B132" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C132" t="inlineStr"/>
@@ -5850,7 +5851,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B133" s="3" t="n">
+      <c r="B133" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C133" t="inlineStr"/>
@@ -5887,7 +5888,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B134" s="3" t="n">
+      <c r="B134" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C134" t="inlineStr"/>
@@ -5924,7 +5925,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B135" s="3" t="n">
+      <c r="B135" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C135" t="inlineStr">
@@ -5965,7 +5966,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvNighthawk</t>
         </is>
       </c>
-      <c r="B136" s="3" t="n">
+      <c r="B136" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C136" t="inlineStr">
@@ -6034,7 +6035,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B137" s="3" t="n">
+      <c r="B137" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -6071,7 +6072,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B138" s="3" t="n">
+      <c r="B138" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C138" t="inlineStr"/>
@@ -6108,7 +6109,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B139" s="3" t="n">
+      <c r="B139" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C139" t="inlineStr"/>
@@ -6145,7 +6146,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B140" s="3" t="n">
+      <c r="B140" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C140" t="inlineStr"/>
@@ -6182,7 +6183,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B141" s="3" t="n">
+      <c r="B141" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C141" t="inlineStr"/>
@@ -6219,7 +6220,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B142" s="3" t="n">
+      <c r="B142" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C142" t="inlineStr"/>
@@ -6256,7 +6257,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B143" s="3" t="n">
+      <c r="B143" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C143" t="inlineStr"/>
@@ -6293,7 +6294,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B144" s="3" t="n">
+      <c r="B144" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C144" t="inlineStr">
@@ -6334,7 +6335,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAnapurna</t>
         </is>
       </c>
-      <c r="B145" s="3" t="n">
+      <c r="B145" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C145" t="inlineStr">
@@ -6403,7 +6404,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B146" s="3" t="n">
+      <c r="B146" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C146" t="inlineStr"/>
@@ -6440,7 +6441,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B147" s="3" t="n">
+      <c r="B147" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C147" t="inlineStr"/>
@@ -6477,7 +6478,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B148" s="3" t="n">
+      <c r="B148" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -6514,7 +6515,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B149" s="3" t="n">
+      <c r="B149" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C149" t="inlineStr"/>
@@ -6551,7 +6552,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B150" s="3" t="n">
+      <c r="B150" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C150" t="inlineStr"/>
@@ -6588,7 +6589,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B151" s="3" t="n">
+      <c r="B151" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C151" t="inlineStr"/>
@@ -6625,7 +6626,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B152" s="3" t="n">
+      <c r="B152" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C152" t="inlineStr"/>
@@ -6662,7 +6663,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B153" s="3" t="n">
+      <c r="B153" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C153" t="inlineStr">
@@ -6703,7 +6704,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvAccroc</t>
         </is>
       </c>
-      <c r="B154" s="3" t="n">
+      <c r="B154" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C154" t="inlineStr">
@@ -6772,7 +6773,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B155" s="3" t="n">
+      <c r="B155" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C155" t="inlineStr"/>
@@ -6809,7 +6810,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B156" s="3" t="n">
+      <c r="B156" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C156" t="inlineStr"/>
@@ -6846,7 +6847,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B157" s="3" t="n">
+      <c r="B157" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C157" t="inlineStr"/>
@@ -6883,7 +6884,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B158" s="3" t="n">
+      <c r="B158" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C158" t="inlineStr"/>
@@ -6920,7 +6921,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B159" s="3" t="n">
+      <c r="B159" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C159" t="inlineStr"/>
@@ -6957,7 +6958,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B160" s="3" t="n">
+      <c r="B160" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C160" t="inlineStr"/>
@@ -6994,7 +6995,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B161" s="3" t="n">
+      <c r="B161" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C161" t="inlineStr"/>
@@ -7031,7 +7032,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B162" s="3" t="n">
+      <c r="B162" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C162" t="inlineStr">
@@ -7072,7 +7073,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCalabro</t>
         </is>
       </c>
-      <c r="B163" s="3" t="n">
+      <c r="B163" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C163" t="inlineStr">
@@ -7141,7 +7142,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B164" s="3" t="n">
+      <c r="B164" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C164" t="inlineStr"/>
@@ -7178,7 +7179,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B165" s="3" t="n">
+      <c r="B165" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C165" t="inlineStr"/>
@@ -7215,7 +7216,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B166" s="3" t="n">
+      <c r="B166" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C166" t="inlineStr"/>
@@ -7252,7 +7253,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B167" s="3" t="n">
+      <c r="B167" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C167" t="inlineStr"/>
@@ -7289,7 +7290,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B168" s="3" t="n">
+      <c r="B168" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C168" t="inlineStr"/>
@@ -7326,7 +7327,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B169" s="3" t="n">
+      <c r="B169" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C169" t="inlineStr"/>
@@ -7363,7 +7364,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B170" s="3" t="n">
+      <c r="B170" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C170" t="inlineStr"/>
@@ -7400,7 +7401,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B171" s="3" t="n">
+      <c r="B171" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C171" t="inlineStr">
@@ -7441,7 +7442,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvCesario</t>
         </is>
       </c>
-      <c r="B172" s="3" t="n">
+      <c r="B172" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C172" t="inlineStr">
@@ -7510,7 +7511,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B173" s="3" t="n">
+      <c r="B173" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C173" t="inlineStr"/>
@@ -7547,7 +7548,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B174" s="3" t="n">
+      <c r="B174" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C174" t="inlineStr"/>
@@ -7584,7 +7585,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B175" s="3" t="n">
+      <c r="B175" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C175" t="inlineStr"/>
@@ -7621,7 +7622,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B176" s="3" t="n">
+      <c r="B176" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C176" t="inlineStr"/>
@@ -7658,7 +7659,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B177" s="3" t="n">
+      <c r="B177" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C177" t="inlineStr"/>
@@ -7695,7 +7696,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B178" s="3" t="n">
+      <c r="B178" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C178" t="inlineStr"/>
@@ -7732,7 +7733,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B179" s="3" t="n">
+      <c r="B179" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C179" t="inlineStr"/>
@@ -7769,7 +7770,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B180" s="3" t="n">
+      <c r="B180" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C180" t="inlineStr">
@@ -7810,7 +7811,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvTabasco</t>
         </is>
       </c>
-      <c r="B181" s="3" t="n">
+      <c r="B181" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C181" t="inlineStr">
@@ -7879,7 +7880,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B182" s="3" t="n">
+      <c r="B182" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C182" t="inlineStr"/>
@@ -7916,7 +7917,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B183" s="3" t="n">
+      <c r="B183" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C183" t="inlineStr"/>
@@ -7953,7 +7954,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B184" s="3" t="n">
+      <c r="B184" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C184" t="inlineStr"/>
@@ -7990,7 +7991,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B185" s="3" t="n">
+      <c r="B185" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C185" t="inlineStr"/>
@@ -8027,7 +8028,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B186" s="3" t="n">
+      <c r="B186" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C186" t="inlineStr"/>
@@ -8064,7 +8065,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B187" s="3" t="n">
+      <c r="B187" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C187" t="inlineStr"/>
@@ -8101,7 +8102,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B188" s="3" t="n">
+      <c r="B188" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C188" t="inlineStr"/>
@@ -8138,7 +8139,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B189" s="3" t="n">
+      <c r="B189" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C189" t="inlineStr">
@@ -8179,7 +8180,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvBennett</t>
         </is>
       </c>
-      <c r="B190" s="3" t="n">
+      <c r="B190" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C190" t="inlineStr">
@@ -8248,7 +8249,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B191" s="3" t="n">
+      <c r="B191" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C191" t="inlineStr"/>
@@ -8285,7 +8286,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B192" s="3" t="n">
+      <c r="B192" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C192" t="inlineStr"/>
@@ -8322,7 +8323,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B193" s="3" t="n">
+      <c r="B193" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C193" t="inlineStr"/>
@@ -8359,7 +8360,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B194" s="3" t="n">
+      <c r="B194" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C194" t="inlineStr"/>
@@ -8396,7 +8397,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B195" s="3" t="n">
+      <c r="B195" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C195" t="inlineStr"/>
@@ -8433,7 +8434,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B196" s="3" t="n">
+      <c r="B196" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C196" t="inlineStr"/>
@@ -8470,7 +8471,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B197" s="3" t="n">
+      <c r="B197" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C197" t="inlineStr"/>
@@ -8507,7 +8508,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B198" s="3" t="n">
+      <c r="B198" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C198" t="inlineStr">
@@ -8548,7 +8549,7 @@
           <t>FAR DMC W20-03MgmtGrazedCvManning</t>
         </is>
       </c>
-      <c r="B199" s="3" t="n">
+      <c r="B199" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C199" t="inlineStr">
@@ -8617,7 +8618,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B200" s="3" t="n">
+      <c r="B200" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C200" t="inlineStr"/>
@@ -8654,7 +8655,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B201" s="3" t="n">
+      <c r="B201" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -8691,7 +8692,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B202" s="3" t="n">
+      <c r="B202" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -8728,7 +8729,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B203" s="3" t="n">
+      <c r="B203" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C203" t="inlineStr"/>
@@ -8765,7 +8766,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B204" s="3" t="n">
+      <c r="B204" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -8802,7 +8803,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B205" s="3" t="n">
+      <c r="B205" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C205" t="inlineStr"/>
@@ -8839,7 +8840,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B206" s="3" t="n">
+      <c r="B206" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C206" t="inlineStr"/>
@@ -8876,7 +8877,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B207" s="3" t="n">
+      <c r="B207" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C207" t="inlineStr">
@@ -8917,7 +8918,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTrojan</t>
         </is>
       </c>
-      <c r="B208" s="3" t="n">
+      <c r="B208" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C208" t="inlineStr">
@@ -8986,7 +8987,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B209" s="3" t="n">
+      <c r="B209" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C209" t="inlineStr"/>
@@ -9023,7 +9024,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B210" s="3" t="n">
+      <c r="B210" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C210" t="inlineStr"/>
@@ -9060,7 +9061,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B211" s="3" t="n">
+      <c r="B211" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C211" t="inlineStr"/>
@@ -9097,7 +9098,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B212" s="3" t="n">
+      <c r="B212" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C212" t="inlineStr"/>
@@ -9134,7 +9135,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B213" s="3" t="n">
+      <c r="B213" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C213" t="inlineStr"/>
@@ -9171,7 +9172,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B214" s="3" t="n">
+      <c r="B214" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C214" t="inlineStr"/>
@@ -9208,7 +9209,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B215" s="3" t="n">
+      <c r="B215" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C215" t="inlineStr"/>
@@ -9245,7 +9246,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B216" s="3" t="n">
+      <c r="B216" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C216" t="inlineStr">
@@ -9286,7 +9287,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvScepter</t>
         </is>
       </c>
-      <c r="B217" s="3" t="n">
+      <c r="B217" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C217" t="inlineStr">
@@ -9355,7 +9356,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B218" s="3" t="n">
+      <c r="B218" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C218" t="inlineStr"/>
@@ -9392,7 +9393,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B219" s="3" t="n">
+      <c r="B219" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C219" t="inlineStr"/>
@@ -9429,7 +9430,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B220" s="3" t="n">
+      <c r="B220" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C220" t="inlineStr"/>
@@ -9466,7 +9467,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B221" s="3" t="n">
+      <c r="B221" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C221" t="inlineStr"/>
@@ -9503,7 +9504,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B222" s="3" t="n">
+      <c r="B222" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C222" t="inlineStr"/>
@@ -9540,7 +9541,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B223" s="3" t="n">
+      <c r="B223" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C223" t="inlineStr"/>
@@ -9577,7 +9578,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B224" s="3" t="n">
+      <c r="B224" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C224" t="inlineStr"/>
@@ -9614,7 +9615,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B225" s="3" t="n">
+      <c r="B225" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C225" t="inlineStr">
@@ -9655,7 +9656,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvNighthawk</t>
         </is>
       </c>
-      <c r="B226" s="3" t="n">
+      <c r="B226" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C226" t="inlineStr">
@@ -9724,7 +9725,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B227" s="3" t="n">
+      <c r="B227" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C227" t="inlineStr"/>
@@ -9761,7 +9762,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B228" s="3" t="n">
+      <c r="B228" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C228" t="inlineStr"/>
@@ -9798,7 +9799,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B229" s="3" t="n">
+      <c r="B229" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C229" t="inlineStr"/>
@@ -9835,7 +9836,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B230" s="3" t="n">
+      <c r="B230" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C230" t="inlineStr"/>
@@ -9872,7 +9873,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B231" s="3" t="n">
+      <c r="B231" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C231" t="inlineStr"/>
@@ -9909,7 +9910,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B232" s="3" t="n">
+      <c r="B232" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C232" t="inlineStr"/>
@@ -9946,7 +9947,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B233" s="3" t="n">
+      <c r="B233" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C233" t="inlineStr"/>
@@ -9983,7 +9984,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B234" s="3" t="n">
+      <c r="B234" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C234" t="inlineStr">
@@ -10024,7 +10025,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAnapurna</t>
         </is>
       </c>
-      <c r="B235" s="3" t="n">
+      <c r="B235" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C235" t="inlineStr">
@@ -10093,7 +10094,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B236" s="3" t="n">
+      <c r="B236" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C236" t="inlineStr"/>
@@ -10130,7 +10131,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B237" s="3" t="n">
+      <c r="B237" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C237" t="inlineStr"/>
@@ -10167,7 +10168,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B238" s="3" t="n">
+      <c r="B238" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C238" t="inlineStr"/>
@@ -10204,7 +10205,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B239" s="3" t="n">
+      <c r="B239" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C239" t="inlineStr"/>
@@ -10241,7 +10242,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B240" s="3" t="n">
+      <c r="B240" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C240" t="inlineStr"/>
@@ -10278,7 +10279,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B241" s="3" t="n">
+      <c r="B241" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C241" t="inlineStr"/>
@@ -10315,7 +10316,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B242" s="3" t="n">
+      <c r="B242" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C242" t="inlineStr"/>
@@ -10352,7 +10353,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B243" s="3" t="n">
+      <c r="B243" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C243" t="inlineStr">
@@ -10393,7 +10394,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvAccroc</t>
         </is>
       </c>
-      <c r="B244" s="3" t="n">
+      <c r="B244" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C244" t="inlineStr">
@@ -10462,7 +10463,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B245" s="3" t="n">
+      <c r="B245" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C245" t="inlineStr"/>
@@ -10499,7 +10500,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B246" s="3" t="n">
+      <c r="B246" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C246" t="inlineStr"/>
@@ -10536,7 +10537,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B247" s="3" t="n">
+      <c r="B247" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C247" t="inlineStr"/>
@@ -10573,7 +10574,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B248" s="3" t="n">
+      <c r="B248" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C248" t="inlineStr"/>
@@ -10610,7 +10611,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B249" s="3" t="n">
+      <c r="B249" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C249" t="inlineStr"/>
@@ -10647,7 +10648,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B250" s="3" t="n">
+      <c r="B250" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C250" t="inlineStr"/>
@@ -10684,7 +10685,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B251" s="3" t="n">
+      <c r="B251" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C251" t="inlineStr"/>
@@ -10721,7 +10722,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B252" s="3" t="n">
+      <c r="B252" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C252" t="inlineStr">
@@ -10762,7 +10763,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCalabro</t>
         </is>
       </c>
-      <c r="B253" s="3" t="n">
+      <c r="B253" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C253" t="inlineStr">
@@ -10831,7 +10832,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B254" s="3" t="n">
+      <c r="B254" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C254" t="inlineStr"/>
@@ -10868,7 +10869,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B255" s="3" t="n">
+      <c r="B255" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C255" t="inlineStr"/>
@@ -10905,7 +10906,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B256" s="3" t="n">
+      <c r="B256" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C256" t="inlineStr"/>
@@ -10942,7 +10943,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B257" s="3" t="n">
+      <c r="B257" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C257" t="inlineStr"/>
@@ -10979,7 +10980,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B258" s="3" t="n">
+      <c r="B258" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C258" t="inlineStr"/>
@@ -11016,7 +11017,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B259" s="3" t="n">
+      <c r="B259" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C259" t="inlineStr"/>
@@ -11053,7 +11054,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B260" s="3" t="n">
+      <c r="B260" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C260" t="inlineStr"/>
@@ -11090,7 +11091,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B261" s="3" t="n">
+      <c r="B261" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C261" t="inlineStr">
@@ -11131,7 +11132,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvCesario</t>
         </is>
       </c>
-      <c r="B262" s="3" t="n">
+      <c r="B262" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C262" t="inlineStr">
@@ -11200,7 +11201,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B263" s="3" t="n">
+      <c r="B263" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C263" t="inlineStr"/>
@@ -11237,7 +11238,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B264" s="3" t="n">
+      <c r="B264" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C264" t="inlineStr"/>
@@ -11274,7 +11275,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B265" s="3" t="n">
+      <c r="B265" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C265" t="inlineStr"/>
@@ -11311,7 +11312,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B266" s="3" t="n">
+      <c r="B266" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C266" t="inlineStr"/>
@@ -11348,7 +11349,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B267" s="3" t="n">
+      <c r="B267" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C267" t="inlineStr"/>
@@ -11385,7 +11386,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B268" s="3" t="n">
+      <c r="B268" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C268" t="inlineStr"/>
@@ -11422,7 +11423,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B269" s="3" t="n">
+      <c r="B269" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C269" t="inlineStr"/>
@@ -11459,7 +11460,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B270" s="3" t="n">
+      <c r="B270" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C270" t="inlineStr">
@@ -11500,7 +11501,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvTabasco</t>
         </is>
       </c>
-      <c r="B271" s="3" t="n">
+      <c r="B271" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C271" t="inlineStr">
@@ -11569,7 +11570,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B272" s="3" t="n">
+      <c r="B272" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C272" t="inlineStr"/>
@@ -11606,7 +11607,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B273" s="3" t="n">
+      <c r="B273" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C273" t="inlineStr"/>
@@ -11643,7 +11644,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B274" s="3" t="n">
+      <c r="B274" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C274" t="inlineStr"/>
@@ -11680,7 +11681,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B275" s="3" t="n">
+      <c r="B275" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C275" t="inlineStr"/>
@@ -11717,7 +11718,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B276" s="3" t="n">
+      <c r="B276" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C276" t="inlineStr"/>
@@ -11754,7 +11755,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B277" s="3" t="n">
+      <c r="B277" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C277" t="inlineStr"/>
@@ -11791,7 +11792,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B278" s="3" t="n">
+      <c r="B278" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C278" t="inlineStr"/>
@@ -11828,7 +11829,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B279" s="3" t="n">
+      <c r="B279" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C279" t="inlineStr">
@@ -11869,7 +11870,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvBennett</t>
         </is>
       </c>
-      <c r="B280" s="3" t="n">
+      <c r="B280" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C280" t="inlineStr">
@@ -11938,7 +11939,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B281" s="3" t="n">
+      <c r="B281" s="4" t="n">
         <v>44026</v>
       </c>
       <c r="C281" t="inlineStr"/>
@@ -11975,7 +11976,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B282" s="3" t="n">
+      <c r="B282" s="4" t="n">
         <v>44041</v>
       </c>
       <c r="C282" t="inlineStr"/>
@@ -12012,7 +12013,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B283" s="3" t="n">
+      <c r="B283" s="4" t="n">
         <v>44068</v>
       </c>
       <c r="C283" t="inlineStr"/>
@@ -12049,7 +12050,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B284" s="3" t="n">
+      <c r="B284" s="4" t="n">
         <v>44082</v>
       </c>
       <c r="C284" t="inlineStr"/>
@@ -12086,7 +12087,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B285" s="3" t="n">
+      <c r="B285" s="4" t="n">
         <v>44097</v>
       </c>
       <c r="C285" t="inlineStr"/>
@@ -12123,7 +12124,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B286" s="3" t="n">
+      <c r="B286" s="4" t="n">
         <v>44110</v>
       </c>
       <c r="C286" t="inlineStr"/>
@@ -12160,7 +12161,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B287" s="3" t="n">
+      <c r="B287" s="4" t="n">
         <v>44139</v>
       </c>
       <c r="C287" t="inlineStr"/>
@@ -12197,7 +12198,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B288" s="3" t="n">
+      <c r="B288" s="4" t="n">
         <v>44152</v>
       </c>
       <c r="C288" t="inlineStr">
@@ -12238,7 +12239,7 @@
           <t>FAR DMC W20-03MgmtHigh InputCvManning</t>
         </is>
       </c>
-      <c r="B289" s="3" t="n">
+      <c r="B289" s="4" t="n">
         <v>44181</v>
       </c>
       <c r="C289" t="inlineStr">

</xml_diff>